<commit_message>
Updated population spreadsheet; organized natural earth data into folder
</commit_message>
<xml_diff>
--- a/antarctica/antarctica.xlsx
+++ b/antarctica/antarctica.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21060" windowHeight="9260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12380" windowHeight="13460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Place</t>
   </si>
@@ -41,27 +41,15 @@
     <t>Japan</t>
   </si>
   <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
-    <t>Italy</t>
-  </si>
-  <si>
     <t>Netherlands</t>
   </si>
   <si>
     <t>Belgium</t>
   </si>
   <si>
-    <t>Great Britain</t>
-  </si>
-  <si>
     <t>Spain</t>
   </si>
   <si>
@@ -84,6 +72,15 @@
   </si>
   <si>
     <t>Permanent Population</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Hungary</t>
   </si>
 </sst>
 </file>
@@ -450,23 +447,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H23"/>
+  <dimension ref="A2:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,19 +466,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -496,51 +479,28 @@
       <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>5400000</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <f>SUM(B8:B23)</f>
-        <v>4539357</v>
+        <f>SUM(B8:B22)</f>
+        <v>4490354</v>
       </c>
       <c r="C5" s="1">
-        <f>SUM(C8:C23)</f>
-        <v>876913551</v>
-      </c>
-      <c r="G5" s="1">
-        <f>SUM(G8:G23)</f>
-        <v>4539357</v>
-      </c>
-      <c r="H5" s="1">
-        <f>SUM(H8:H23)</f>
-        <v>876913551</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <f>SUM(C8:C22)</f>
+        <v>825592513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>32386</v>
@@ -548,19 +508,10 @@
       <c r="C8" s="1">
         <v>8794267</v>
       </c>
-      <c r="F8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="G8" s="1">
-        <v>32386</v>
-      </c>
-      <c r="H8" s="1">
-        <v>8794267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>11787</v>
@@ -568,37 +519,21 @@
       <c r="C9" s="1">
         <v>11303528</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1">
-        <v>11787</v>
-      </c>
-      <c r="H9" s="1">
-        <v>11303528</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
-        <v>213011</v>
+        <f>213011-3350</f>
+        <v>209661</v>
       </c>
       <c r="C10" s="1">
-        <v>65058000</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="1">
-        <v>213011</v>
-      </c>
-      <c r="H10" s="1">
-        <v>65058000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <f>65058000-330000</f>
+        <v>64728000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>3</v>
       </c>
@@ -608,39 +543,21 @@
       <c r="C11" s="1">
         <v>82800000</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="1">
-        <v>137903</v>
-      </c>
-      <c r="H11" s="1">
-        <v>82800000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
         <v>93628</v>
       </c>
       <c r="C12" s="1">
-        <v>60800000</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="1">
-        <v>93628</v>
-      </c>
-      <c r="H12" s="1">
-        <v>60800000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>65648100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
         <v>32595</v>
@@ -648,222 +565,108 @@
       <c r="C13" s="1">
         <v>6572728</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="1">
-        <v>32595</v>
-      </c>
-      <c r="H13" s="1">
-        <v>6572728</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1">
+        <v>145936</v>
+      </c>
+      <c r="C14" s="1">
+        <v>126672000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>16040</v>
+      </c>
+      <c r="C15" s="1">
+        <v>17170000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
+        <v>148728</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5267146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1">
+        <v>120726</v>
+      </c>
+      <c r="C17" s="1">
+        <v>38422346</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1">
-        <v>116347</v>
-      </c>
-      <c r="C14" s="1">
-        <v>60589445</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="1">
-        <v>116347</v>
-      </c>
-      <c r="H14" s="1">
-        <v>60589445</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1">
-        <v>145936</v>
-      </c>
-      <c r="C15" s="1">
-        <v>126672000</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" s="1">
-        <v>145936</v>
-      </c>
-      <c r="H15" s="1">
-        <v>126672000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="B18" s="1">
+        <v>195360</v>
+      </c>
+      <c r="C18" s="1">
+        <v>46354321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="1">
-        <v>16040</v>
-      </c>
-      <c r="C16" s="1">
-        <v>17170000</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="1">
-        <v>16040</v>
-      </c>
-      <c r="H16" s="1">
-        <v>17170000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1">
-        <v>103483</v>
-      </c>
-      <c r="C17" s="1">
-        <v>4850350</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="1">
-        <v>103483</v>
-      </c>
-      <c r="H17" s="1">
-        <v>4850350</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="1">
-        <v>148728</v>
-      </c>
-      <c r="C18" s="1">
-        <v>5267146</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="1">
-        <v>148728</v>
-      </c>
-      <c r="H18" s="1">
-        <v>5267146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="B19" s="1">
-        <v>120726</v>
+        <v>15940</v>
       </c>
       <c r="C19" s="1">
-        <v>38422346</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="1">
-        <v>120726</v>
-      </c>
-      <c r="H19" s="1">
-        <v>38422346</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8401120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1">
-        <v>35603</v>
+        <v>12</v>
+      </c>
+      <c r="B20" s="4">
+        <v>3119884</v>
       </c>
       <c r="C20" s="1">
-        <v>10309573</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="1">
-        <v>35603</v>
-      </c>
-      <c r="H20" s="1">
-        <v>10309573</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="1">
-        <v>195360</v>
-      </c>
-      <c r="C21" s="1">
-        <v>46354321</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="1">
-        <v>195360</v>
-      </c>
-      <c r="H21" s="1">
-        <v>46354321</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="1">
-        <v>15940</v>
-      </c>
-      <c r="C22" s="1">
-        <v>8401120</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="1">
-        <v>15940</v>
-      </c>
-      <c r="H22" s="1">
-        <v>8401120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="4">
-        <v>3119884</v>
-      </c>
-      <c r="C23" s="1">
         <f>325719178-741894-1428557</f>
         <v>323548727</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="4">
-        <v>3119884</v>
-      </c>
-      <c r="H23" s="1">
-        <f>325719178-741894-1428557</f>
-        <v>323548727</v>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1">
+        <v>35920</v>
+      </c>
+      <c r="C21" s="1">
+        <v>9797561</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1">
+        <v>173860</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10112669</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A8:B24">
-    <sortCondition ref="A21"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>